<commit_message>
Changes to Module 8-10
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_8_10.xlsx
+++ b/templates/NHWA_Module_8_10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20351"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8F78F1-C2EE-4169-B4C5-BB06FA3E12CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62B622A-C58C-4AF3-A049-ED6A492CF972}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="zzB/EG68cBLCavBKifLXLU9cHtkByNHDxKw6TGAOmH0Xqt9eEqslmxhiS3RNT5/yg3W/p9o2mkoBv+FWclA2/Q==" workbookSaltValue="AdDK0FT/Ht0UdvlaiqFRnA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -2656,6 +2656,16 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2665,16 +2675,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4137,16 +4137,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -4177,16 +4177,16 @@
       </c>
     </row>
     <row r="2" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="38" t="s">
         <v>761</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -4365,29 +4365,29 @@
       </c>
     </row>
     <row r="6" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="37" t="s">
         <v>759</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="37" t="s">
         <v>762</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="37" t="s">
         <v>782</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="14"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
       <c r="V6" s="4" t="s">
         <v>787</v>
       </c>
@@ -4417,13 +4417,13 @@
       </c>
     </row>
     <row r="7" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="14"/>
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
@@ -4469,10 +4469,10 @@
         <v>783</v>
       </c>
       <c r="D8" s="34"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
       <c r="I8" s="14"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
@@ -4512,10 +4512,10 @@
         <v>784</v>
       </c>
       <c r="D9" s="34"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
       <c r="I9" s="14"/>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
@@ -4555,10 +4555,10 @@
         <v>785</v>
       </c>
       <c r="D10" s="35"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
       <c r="I10" s="14"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -4604,10 +4604,10 @@
         <v>765</v>
       </c>
       <c r="D11" s="35"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
       <c r="I11" s="14"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
@@ -4651,10 +4651,10 @@
         <v>786</v>
       </c>
       <c r="D12" s="35"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
       <c r="I12" s="14"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
@@ -4705,10 +4705,10 @@
         <v>763</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="14"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
@@ -4762,10 +4762,10 @@
         <v>764</v>
       </c>
       <c r="D14" s="22"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
       <c r="I14" s="14"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
@@ -4809,10 +4809,10 @@
         <v>765</v>
       </c>
       <c r="D15" s="22"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="14"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
@@ -11031,19 +11031,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ayvvL4B0rTmiFtoL19BmlgzP+5zKbPPR9GO1TrkLAaTIwNt3IeEuZgbylSBRZXxwEKB3feYmUw1a6fmT88kPKQ==" saltValue="DJoPVZM/QTKyvsO1jcr2Qg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="YA4PVbikWZ2/m0THKQhwV3mqAEgRR8xmtWfDcLhl4xKzO+0hA8Hpaek/5/A3MsTKQ/LsxRdQRh2NfAV8cYg0lw==" saltValue="u3mFMoVoOnf9WzPwuSf3Fg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="I4 Q8:R16 F8:P10 F14:P14 G11:P13 H15:P15 D17:G17 D21:G21 F13" name="Range1"/>
     <protectedRange sqref="D10:E13" name="Range1_1"/>
   </protectedRanges>
   <mergeCells count="15">
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="E6:H7"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E13:H13"/>
@@ -11052,6 +11045,13 @@
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="E11:H11"/>
     <mergeCell ref="E12:H12"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="E6:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11182,32 +11182,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="2:19" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="38" t="s">
         <v>767</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -11272,33 +11272,33 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="37" t="s">
         <v>759</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="37" t="s">
         <v>766</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="37" t="s">
         <v>782</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="2:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="N8" s="9"/>
       <c r="Q8" s="4" t="s">
         <v>757</v>
@@ -11476,17 +11476,17 @@
     <protectedRange sqref="D9:D11 D14" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="11">
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:I8"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11640,32 +11640,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="2:19" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="38" t="s">
         <v>773</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -11730,31 +11730,31 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="37" t="s">
         <v>759</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="37" t="s">
         <v>766</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="37" t="s">
         <v>782</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="2:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
       <c r="N8" s="9"/>
       <c r="Q8" s="4" t="s">
         <v>788</v>
@@ -12011,12 +12011,6 @@
     <protectedRange sqref="D9:D11 D14" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="14">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:H8"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E16:H16"/>
@@ -12025,6 +12019,12 @@
     <mergeCell ref="E11:H11"/>
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="E13:H13"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>